<commit_message>
Created a conditions file and started coding the presentation phase.
</commit_message>
<xml_diff>
--- a/cond-files/cond_pm1.xlsx
+++ b/cond-files/cond_pm1.xlsx
@@ -1,31 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Egor\Dropbox\Projects\eb\eb\cond-files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egora\Dropbox\Projects\pm\pm\cond-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E1FD737-45CF-440E-93E2-F95BF088EE0A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C061406-3572-4263-8D26-E21B7EB03DAA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="92" yWindow="144" windowWidth="16259" windowHeight="5590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="cond_eb1_c" sheetId="1" r:id="rId1"/>
+    <sheet name="cond_pm1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>targ_right</t>
+    <t>stim1_c</t>
   </si>
   <si>
-    <t>cue_valid</t>
+    <t>stim2_c</t>
+  </si>
+  <si>
+    <t>SOA</t>
+  </si>
+  <si>
+    <t>angle_diff</t>
   </si>
 </sst>
 </file>
@@ -891,84 +897,2714 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:D193"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A98" sqref="A98:A193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2">
+        <v>-2</v>
+      </c>
+      <c r="D2">
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0</v>
       </c>
       <c r="B3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>-2</v>
+      </c>
+      <c r="D3">
+        <v>-1.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0</v>
       </c>
       <c r="B4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>-2</v>
+      </c>
+      <c r="D4">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0</v>
       </c>
       <c r="B5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>-2</v>
+      </c>
+      <c r="D5">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>-1.6</v>
+      </c>
+      <c r="D6">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>-1.6</v>
+      </c>
+      <c r="D7">
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>-1.6</v>
+      </c>
+      <c r="D8">
+        <v>-1.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>-1.6</v>
+      </c>
+      <c r="D9">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>-1.6</v>
+      </c>
+      <c r="D10">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>-1.2</v>
+      </c>
+      <c r="D11">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>-1.2</v>
+      </c>
+      <c r="D12">
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>-1.2</v>
+      </c>
+      <c r="D13">
+        <v>-1.2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>-1.2</v>
+      </c>
+      <c r="D14">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>-1.2</v>
+      </c>
+      <c r="D15">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>-0.8</v>
+      </c>
+      <c r="D16">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>-0.8</v>
+      </c>
+      <c r="D17">
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>-0.8</v>
+      </c>
+      <c r="D18">
+        <v>-1.2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>0</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>-0.8</v>
+      </c>
+      <c r="D19">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>0</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>-0.8</v>
+      </c>
+      <c r="D20">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>0</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>-0.4</v>
+      </c>
+      <c r="D21">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>0</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>-0.4</v>
+      </c>
+      <c r="D22">
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>0</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>-0.4</v>
+      </c>
+      <c r="D23">
+        <v>-1.2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>0</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>-0.4</v>
+      </c>
+      <c r="D24">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>0</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>-0.4</v>
+      </c>
+      <c r="D25">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>0</v>
+      </c>
+      <c r="B26">
+        <v>20</v>
+      </c>
+      <c r="C26">
+        <v>-2</v>
+      </c>
+      <c r="D26">
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>0</v>
+      </c>
+      <c r="B27">
+        <v>20</v>
+      </c>
+      <c r="C27">
+        <v>-2</v>
+      </c>
+      <c r="D27">
+        <v>-1.2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>0</v>
+      </c>
+      <c r="B28">
+        <v>20</v>
+      </c>
+      <c r="C28">
+        <v>-2</v>
+      </c>
+      <c r="D28">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>0</v>
+      </c>
+      <c r="B29">
+        <v>20</v>
+      </c>
+      <c r="C29">
+        <v>-2</v>
+      </c>
+      <c r="D29">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>0</v>
+      </c>
+      <c r="B30">
+        <v>20</v>
+      </c>
+      <c r="C30">
+        <v>-1.6</v>
+      </c>
+      <c r="D30">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>0</v>
+      </c>
+      <c r="B31">
+        <v>20</v>
+      </c>
+      <c r="C31">
+        <v>-1.6</v>
+      </c>
+      <c r="D31">
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>0</v>
+      </c>
+      <c r="B32">
+        <v>20</v>
+      </c>
+      <c r="C32">
+        <v>-1.6</v>
+      </c>
+      <c r="D32">
+        <v>-1.2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>0</v>
+      </c>
+      <c r="B33">
+        <v>20</v>
+      </c>
+      <c r="C33">
+        <v>-1.6</v>
+      </c>
+      <c r="D33">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>0</v>
+      </c>
+      <c r="B34">
+        <v>20</v>
+      </c>
+      <c r="C34">
+        <v>-1.6</v>
+      </c>
+      <c r="D34">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>0</v>
+      </c>
+      <c r="B35">
+        <v>20</v>
+      </c>
+      <c r="C35">
+        <v>-1.2</v>
+      </c>
+      <c r="D35">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>0</v>
+      </c>
+      <c r="B36">
+        <v>20</v>
+      </c>
+      <c r="C36">
+        <v>-1.2</v>
+      </c>
+      <c r="D36">
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>0</v>
+      </c>
+      <c r="B37">
+        <v>20</v>
+      </c>
+      <c r="C37">
+        <v>-1.2</v>
+      </c>
+      <c r="D37">
+        <v>-1.2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>0</v>
+      </c>
+      <c r="B38">
+        <v>20</v>
+      </c>
+      <c r="C38">
+        <v>-1.2</v>
+      </c>
+      <c r="D38">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>0</v>
+      </c>
+      <c r="B39">
+        <v>20</v>
+      </c>
+      <c r="C39">
+        <v>-1.2</v>
+      </c>
+      <c r="D39">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>0</v>
+      </c>
+      <c r="B40">
+        <v>20</v>
+      </c>
+      <c r="C40">
+        <v>-0.8</v>
+      </c>
+      <c r="D40">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>0</v>
+      </c>
+      <c r="B41">
+        <v>20</v>
+      </c>
+      <c r="C41">
+        <v>-0.8</v>
+      </c>
+      <c r="D41">
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>0</v>
+      </c>
+      <c r="B42">
+        <v>20</v>
+      </c>
+      <c r="C42">
+        <v>-0.8</v>
+      </c>
+      <c r="D42">
+        <v>-1.2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>0</v>
+      </c>
+      <c r="B43">
+        <v>20</v>
+      </c>
+      <c r="C43">
+        <v>-0.8</v>
+      </c>
+      <c r="D43">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>0</v>
+      </c>
+      <c r="B44">
+        <v>20</v>
+      </c>
+      <c r="C44">
+        <v>-0.8</v>
+      </c>
+      <c r="D44">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>0</v>
+      </c>
+      <c r="B45">
+        <v>20</v>
+      </c>
+      <c r="C45">
+        <v>-0.4</v>
+      </c>
+      <c r="D45">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>0</v>
+      </c>
+      <c r="B46">
+        <v>20</v>
+      </c>
+      <c r="C46">
+        <v>-0.4</v>
+      </c>
+      <c r="D46">
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>0</v>
+      </c>
+      <c r="B47">
+        <v>20</v>
+      </c>
+      <c r="C47">
+        <v>-0.4</v>
+      </c>
+      <c r="D47">
+        <v>-1.2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>0</v>
+      </c>
+      <c r="B48">
+        <v>20</v>
+      </c>
+      <c r="C48">
+        <v>-0.4</v>
+      </c>
+      <c r="D48">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>0</v>
+      </c>
+      <c r="B49">
+        <v>20</v>
+      </c>
+      <c r="C49">
+        <v>-0.4</v>
+      </c>
+      <c r="D49">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>0</v>
+      </c>
+      <c r="B50">
+        <v>60</v>
+      </c>
+      <c r="C50">
+        <v>-2</v>
+      </c>
+      <c r="D50">
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>0</v>
+      </c>
+      <c r="B51">
+        <v>60</v>
+      </c>
+      <c r="C51">
+        <v>-2</v>
+      </c>
+      <c r="D51">
+        <v>-1.2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>0</v>
+      </c>
+      <c r="B52">
+        <v>60</v>
+      </c>
+      <c r="C52">
+        <v>-2</v>
+      </c>
+      <c r="D52">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>0</v>
+      </c>
+      <c r="B53">
+        <v>60</v>
+      </c>
+      <c r="C53">
+        <v>-2</v>
+      </c>
+      <c r="D53">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>0</v>
+      </c>
+      <c r="B54">
+        <v>60</v>
+      </c>
+      <c r="C54">
+        <v>-1.6</v>
+      </c>
+      <c r="D54">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>0</v>
+      </c>
+      <c r="B55">
+        <v>60</v>
+      </c>
+      <c r="C55">
+        <v>-1.6</v>
+      </c>
+      <c r="D55">
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>0</v>
+      </c>
+      <c r="B56">
+        <v>60</v>
+      </c>
+      <c r="C56">
+        <v>-1.6</v>
+      </c>
+      <c r="D56">
+        <v>-1.2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>0</v>
+      </c>
+      <c r="B57">
+        <v>60</v>
+      </c>
+      <c r="C57">
+        <v>-1.6</v>
+      </c>
+      <c r="D57">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>0</v>
+      </c>
+      <c r="B58">
+        <v>60</v>
+      </c>
+      <c r="C58">
+        <v>-1.6</v>
+      </c>
+      <c r="D58">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>0</v>
+      </c>
+      <c r="B59">
+        <v>60</v>
+      </c>
+      <c r="C59">
+        <v>-1.2</v>
+      </c>
+      <c r="D59">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>0</v>
+      </c>
+      <c r="B60">
+        <v>60</v>
+      </c>
+      <c r="C60">
+        <v>-1.2</v>
+      </c>
+      <c r="D60">
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>0</v>
+      </c>
+      <c r="B61">
+        <v>60</v>
+      </c>
+      <c r="C61">
+        <v>-1.2</v>
+      </c>
+      <c r="D61">
+        <v>-1.2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>0</v>
+      </c>
+      <c r="B62">
+        <v>60</v>
+      </c>
+      <c r="C62">
+        <v>-1.2</v>
+      </c>
+      <c r="D62">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>0</v>
+      </c>
+      <c r="B63">
+        <v>60</v>
+      </c>
+      <c r="C63">
+        <v>-1.2</v>
+      </c>
+      <c r="D63">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>0</v>
+      </c>
+      <c r="B64">
+        <v>60</v>
+      </c>
+      <c r="C64">
+        <v>-0.8</v>
+      </c>
+      <c r="D64">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>0</v>
+      </c>
+      <c r="B65">
+        <v>60</v>
+      </c>
+      <c r="C65">
+        <v>-0.8</v>
+      </c>
+      <c r="D65">
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>0</v>
+      </c>
+      <c r="B66">
+        <v>60</v>
+      </c>
+      <c r="C66">
+        <v>-0.8</v>
+      </c>
+      <c r="D66">
+        <v>-1.2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>0</v>
+      </c>
+      <c r="B67">
+        <v>60</v>
+      </c>
+      <c r="C67">
+        <v>-0.8</v>
+      </c>
+      <c r="D67">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>0</v>
+      </c>
+      <c r="B68">
+        <v>60</v>
+      </c>
+      <c r="C68">
+        <v>-0.8</v>
+      </c>
+      <c r="D68">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>0</v>
+      </c>
+      <c r="B69">
+        <v>60</v>
+      </c>
+      <c r="C69">
+        <v>-0.4</v>
+      </c>
+      <c r="D69">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>0</v>
+      </c>
+      <c r="B70">
+        <v>60</v>
+      </c>
+      <c r="C70">
+        <v>-0.4</v>
+      </c>
+      <c r="D70">
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>0</v>
+      </c>
+      <c r="B71">
+        <v>60</v>
+      </c>
+      <c r="C71">
+        <v>-0.4</v>
+      </c>
+      <c r="D71">
+        <v>-1.2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>0</v>
+      </c>
+      <c r="B72">
+        <v>60</v>
+      </c>
+      <c r="C72">
+        <v>-0.4</v>
+      </c>
+      <c r="D72">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>0</v>
+      </c>
+      <c r="B73">
+        <v>60</v>
+      </c>
+      <c r="C73">
+        <v>-0.4</v>
+      </c>
+      <c r="D73">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>0</v>
+      </c>
+      <c r="B74">
+        <v>120</v>
+      </c>
+      <c r="C74">
+        <v>-2</v>
+      </c>
+      <c r="D74">
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>0</v>
+      </c>
+      <c r="B75">
+        <v>120</v>
+      </c>
+      <c r="C75">
+        <v>-2</v>
+      </c>
+      <c r="D75">
+        <v>-1.2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>0</v>
+      </c>
+      <c r="B76">
+        <v>120</v>
+      </c>
+      <c r="C76">
+        <v>-2</v>
+      </c>
+      <c r="D76">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>0</v>
+      </c>
+      <c r="B77">
+        <v>120</v>
+      </c>
+      <c r="C77">
+        <v>-2</v>
+      </c>
+      <c r="D77">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>0</v>
+      </c>
+      <c r="B78">
+        <v>120</v>
+      </c>
+      <c r="C78">
+        <v>-1.6</v>
+      </c>
+      <c r="D78">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>0</v>
+      </c>
+      <c r="B79">
+        <v>120</v>
+      </c>
+      <c r="C79">
+        <v>-1.6</v>
+      </c>
+      <c r="D79">
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>0</v>
+      </c>
+      <c r="B80">
+        <v>120</v>
+      </c>
+      <c r="C80">
+        <v>-1.6</v>
+      </c>
+      <c r="D80">
+        <v>-1.2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>0</v>
+      </c>
+      <c r="B81">
+        <v>120</v>
+      </c>
+      <c r="C81">
+        <v>-1.6</v>
+      </c>
+      <c r="D81">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>0</v>
+      </c>
+      <c r="B82">
+        <v>120</v>
+      </c>
+      <c r="C82">
+        <v>-1.6</v>
+      </c>
+      <c r="D82">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>0</v>
+      </c>
+      <c r="B83">
+        <v>120</v>
+      </c>
+      <c r="C83">
+        <v>-1.2</v>
+      </c>
+      <c r="D83">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>0</v>
+      </c>
+      <c r="B84">
+        <v>120</v>
+      </c>
+      <c r="C84">
+        <v>-1.2</v>
+      </c>
+      <c r="D84">
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>0</v>
+      </c>
+      <c r="B85">
+        <v>120</v>
+      </c>
+      <c r="C85">
+        <v>-1.2</v>
+      </c>
+      <c r="D85">
+        <v>-1.2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>0</v>
+      </c>
+      <c r="B86">
+        <v>120</v>
+      </c>
+      <c r="C86">
+        <v>-1.2</v>
+      </c>
+      <c r="D86">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>0</v>
+      </c>
+      <c r="B87">
+        <v>120</v>
+      </c>
+      <c r="C87">
+        <v>-1.2</v>
+      </c>
+      <c r="D87">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>0</v>
+      </c>
+      <c r="B88">
+        <v>120</v>
+      </c>
+      <c r="C88">
+        <v>-0.8</v>
+      </c>
+      <c r="D88">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>0</v>
+      </c>
+      <c r="B89">
+        <v>120</v>
+      </c>
+      <c r="C89">
+        <v>-0.8</v>
+      </c>
+      <c r="D89">
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>0</v>
+      </c>
+      <c r="B90">
+        <v>120</v>
+      </c>
+      <c r="C90">
+        <v>-0.8</v>
+      </c>
+      <c r="D90">
+        <v>-1.2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>0</v>
+      </c>
+      <c r="B91">
+        <v>120</v>
+      </c>
+      <c r="C91">
+        <v>-0.8</v>
+      </c>
+      <c r="D91">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>0</v>
+      </c>
+      <c r="B92">
+        <v>120</v>
+      </c>
+      <c r="C92">
+        <v>-0.8</v>
+      </c>
+      <c r="D92">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>0</v>
+      </c>
+      <c r="B93">
+        <v>120</v>
+      </c>
+      <c r="C93">
+        <v>-0.4</v>
+      </c>
+      <c r="D93">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>0</v>
+      </c>
+      <c r="B94">
+        <v>120</v>
+      </c>
+      <c r="C94">
+        <v>-0.4</v>
+      </c>
+      <c r="D94">
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>0</v>
+      </c>
+      <c r="B95">
+        <v>120</v>
+      </c>
+      <c r="C95">
+        <v>-0.4</v>
+      </c>
+      <c r="D95">
+        <v>-1.2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>0</v>
+      </c>
+      <c r="B96">
+        <v>120</v>
+      </c>
+      <c r="C96">
+        <v>-0.4</v>
+      </c>
+      <c r="D96">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>0</v>
+      </c>
+      <c r="B97">
+        <v>120</v>
+      </c>
+      <c r="C97">
+        <v>-0.4</v>
+      </c>
+      <c r="D97">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>1</v>
+      </c>
+      <c r="B98">
+        <v>0</v>
+      </c>
+      <c r="C98">
+        <v>-2</v>
+      </c>
+      <c r="D98">
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <v>1</v>
+      </c>
+      <c r="B99">
+        <v>0</v>
+      </c>
+      <c r="C99">
+        <v>-2</v>
+      </c>
+      <c r="D99">
+        <v>-1.2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <v>1</v>
+      </c>
+      <c r="B100">
+        <v>0</v>
+      </c>
+      <c r="C100">
+        <v>-2</v>
+      </c>
+      <c r="D100">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <v>1</v>
+      </c>
+      <c r="B101">
+        <v>0</v>
+      </c>
+      <c r="C101">
+        <v>-2</v>
+      </c>
+      <c r="D101">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <v>1</v>
+      </c>
+      <c r="B102">
+        <v>0</v>
+      </c>
+      <c r="C102">
+        <v>-1.6</v>
+      </c>
+      <c r="D102">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A103">
+        <v>1</v>
+      </c>
+      <c r="B103">
+        <v>0</v>
+      </c>
+      <c r="C103">
+        <v>-1.6</v>
+      </c>
+      <c r="D103">
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A104">
+        <v>1</v>
+      </c>
+      <c r="B104">
+        <v>0</v>
+      </c>
+      <c r="C104">
+        <v>-1.6</v>
+      </c>
+      <c r="D104">
+        <v>-1.2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A105">
+        <v>1</v>
+      </c>
+      <c r="B105">
+        <v>0</v>
+      </c>
+      <c r="C105">
+        <v>-1.6</v>
+      </c>
+      <c r="D105">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A106">
+        <v>1</v>
+      </c>
+      <c r="B106">
+        <v>0</v>
+      </c>
+      <c r="C106">
+        <v>-1.6</v>
+      </c>
+      <c r="D106">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A107">
+        <v>1</v>
+      </c>
+      <c r="B107">
+        <v>0</v>
+      </c>
+      <c r="C107">
+        <v>-1.2</v>
+      </c>
+      <c r="D107">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A108">
+        <v>1</v>
+      </c>
+      <c r="B108">
+        <v>0</v>
+      </c>
+      <c r="C108">
+        <v>-1.2</v>
+      </c>
+      <c r="D108">
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A109">
+        <v>1</v>
+      </c>
+      <c r="B109">
+        <v>0</v>
+      </c>
+      <c r="C109">
+        <v>-1.2</v>
+      </c>
+      <c r="D109">
+        <v>-1.2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A110">
+        <v>1</v>
+      </c>
+      <c r="B110">
+        <v>0</v>
+      </c>
+      <c r="C110">
+        <v>-1.2</v>
+      </c>
+      <c r="D110">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A111">
+        <v>1</v>
+      </c>
+      <c r="B111">
+        <v>0</v>
+      </c>
+      <c r="C111">
+        <v>-1.2</v>
+      </c>
+      <c r="D111">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A112">
+        <v>1</v>
+      </c>
+      <c r="B112">
+        <v>0</v>
+      </c>
+      <c r="C112">
+        <v>-0.8</v>
+      </c>
+      <c r="D112">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A113">
+        <v>1</v>
+      </c>
+      <c r="B113">
+        <v>0</v>
+      </c>
+      <c r="C113">
+        <v>-0.8</v>
+      </c>
+      <c r="D113">
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A114">
+        <v>1</v>
+      </c>
+      <c r="B114">
+        <v>0</v>
+      </c>
+      <c r="C114">
+        <v>-0.8</v>
+      </c>
+      <c r="D114">
+        <v>-1.2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A115">
+        <v>1</v>
+      </c>
+      <c r="B115">
+        <v>0</v>
+      </c>
+      <c r="C115">
+        <v>-0.8</v>
+      </c>
+      <c r="D115">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A116">
+        <v>1</v>
+      </c>
+      <c r="B116">
+        <v>0</v>
+      </c>
+      <c r="C116">
+        <v>-0.8</v>
+      </c>
+      <c r="D116">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A117">
+        <v>1</v>
+      </c>
+      <c r="B117">
+        <v>0</v>
+      </c>
+      <c r="C117">
+        <v>-0.4</v>
+      </c>
+      <c r="D117">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A118">
+        <v>1</v>
+      </c>
+      <c r="B118">
+        <v>0</v>
+      </c>
+      <c r="C118">
+        <v>-0.4</v>
+      </c>
+      <c r="D118">
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A119">
+        <v>1</v>
+      </c>
+      <c r="B119">
+        <v>0</v>
+      </c>
+      <c r="C119">
+        <v>-0.4</v>
+      </c>
+      <c r="D119">
+        <v>-1.2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A120">
+        <v>1</v>
+      </c>
+      <c r="B120">
+        <v>0</v>
+      </c>
+      <c r="C120">
+        <v>-0.4</v>
+      </c>
+      <c r="D120">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A121">
+        <v>1</v>
+      </c>
+      <c r="B121">
+        <v>0</v>
+      </c>
+      <c r="C121">
+        <v>-0.4</v>
+      </c>
+      <c r="D121">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A122">
+        <v>1</v>
+      </c>
+      <c r="B122">
+        <v>20</v>
+      </c>
+      <c r="C122">
+        <v>-2</v>
+      </c>
+      <c r="D122">
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A123">
+        <v>1</v>
+      </c>
+      <c r="B123">
+        <v>20</v>
+      </c>
+      <c r="C123">
+        <v>-2</v>
+      </c>
+      <c r="D123">
+        <v>-1.2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A124">
+        <v>1</v>
+      </c>
+      <c r="B124">
+        <v>20</v>
+      </c>
+      <c r="C124">
+        <v>-2</v>
+      </c>
+      <c r="D124">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A125">
+        <v>1</v>
+      </c>
+      <c r="B125">
+        <v>20</v>
+      </c>
+      <c r="C125">
+        <v>-2</v>
+      </c>
+      <c r="D125">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A126">
+        <v>1</v>
+      </c>
+      <c r="B126">
+        <v>20</v>
+      </c>
+      <c r="C126">
+        <v>-1.6</v>
+      </c>
+      <c r="D126">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A127">
+        <v>1</v>
+      </c>
+      <c r="B127">
+        <v>20</v>
+      </c>
+      <c r="C127">
+        <v>-1.6</v>
+      </c>
+      <c r="D127">
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A128">
+        <v>1</v>
+      </c>
+      <c r="B128">
+        <v>20</v>
+      </c>
+      <c r="C128">
+        <v>-1.6</v>
+      </c>
+      <c r="D128">
+        <v>-1.2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A129">
+        <v>1</v>
+      </c>
+      <c r="B129">
+        <v>20</v>
+      </c>
+      <c r="C129">
+        <v>-1.6</v>
+      </c>
+      <c r="D129">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A130">
+        <v>1</v>
+      </c>
+      <c r="B130">
+        <v>20</v>
+      </c>
+      <c r="C130">
+        <v>-1.6</v>
+      </c>
+      <c r="D130">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A131">
+        <v>1</v>
+      </c>
+      <c r="B131">
+        <v>20</v>
+      </c>
+      <c r="C131">
+        <v>-1.2</v>
+      </c>
+      <c r="D131">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A132">
+        <v>1</v>
+      </c>
+      <c r="B132">
+        <v>20</v>
+      </c>
+      <c r="C132">
+        <v>-1.2</v>
+      </c>
+      <c r="D132">
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A133">
+        <v>1</v>
+      </c>
+      <c r="B133">
+        <v>20</v>
+      </c>
+      <c r="C133">
+        <v>-1.2</v>
+      </c>
+      <c r="D133">
+        <v>-1.2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A134">
+        <v>1</v>
+      </c>
+      <c r="B134">
+        <v>20</v>
+      </c>
+      <c r="C134">
+        <v>-1.2</v>
+      </c>
+      <c r="D134">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A135">
+        <v>1</v>
+      </c>
+      <c r="B135">
+        <v>20</v>
+      </c>
+      <c r="C135">
+        <v>-1.2</v>
+      </c>
+      <c r="D135">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A136">
+        <v>1</v>
+      </c>
+      <c r="B136">
+        <v>20</v>
+      </c>
+      <c r="C136">
+        <v>-0.8</v>
+      </c>
+      <c r="D136">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A137">
+        <v>1</v>
+      </c>
+      <c r="B137">
+        <v>20</v>
+      </c>
+      <c r="C137">
+        <v>-0.8</v>
+      </c>
+      <c r="D137">
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A138">
+        <v>1</v>
+      </c>
+      <c r="B138">
+        <v>20</v>
+      </c>
+      <c r="C138">
+        <v>-0.8</v>
+      </c>
+      <c r="D138">
+        <v>-1.2</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A139">
+        <v>1</v>
+      </c>
+      <c r="B139">
+        <v>20</v>
+      </c>
+      <c r="C139">
+        <v>-0.8</v>
+      </c>
+      <c r="D139">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A140">
+        <v>1</v>
+      </c>
+      <c r="B140">
+        <v>20</v>
+      </c>
+      <c r="C140">
+        <v>-0.8</v>
+      </c>
+      <c r="D140">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A141">
+        <v>1</v>
+      </c>
+      <c r="B141">
+        <v>20</v>
+      </c>
+      <c r="C141">
+        <v>-0.4</v>
+      </c>
+      <c r="D141">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A142">
+        <v>1</v>
+      </c>
+      <c r="B142">
+        <v>20</v>
+      </c>
+      <c r="C142">
+        <v>-0.4</v>
+      </c>
+      <c r="D142">
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A143">
+        <v>1</v>
+      </c>
+      <c r="B143">
+        <v>20</v>
+      </c>
+      <c r="C143">
+        <v>-0.4</v>
+      </c>
+      <c r="D143">
+        <v>-1.2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A144">
+        <v>1</v>
+      </c>
+      <c r="B144">
+        <v>20</v>
+      </c>
+      <c r="C144">
+        <v>-0.4</v>
+      </c>
+      <c r="D144">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A145">
+        <v>1</v>
+      </c>
+      <c r="B145">
+        <v>20</v>
+      </c>
+      <c r="C145">
+        <v>-0.4</v>
+      </c>
+      <c r="D145">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A146">
+        <v>1</v>
+      </c>
+      <c r="B146">
+        <v>60</v>
+      </c>
+      <c r="C146">
+        <v>-2</v>
+      </c>
+      <c r="D146">
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A147">
+        <v>1</v>
+      </c>
+      <c r="B147">
+        <v>60</v>
+      </c>
+      <c r="C147">
+        <v>-2</v>
+      </c>
+      <c r="D147">
+        <v>-1.2</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A148">
+        <v>1</v>
+      </c>
+      <c r="B148">
+        <v>60</v>
+      </c>
+      <c r="C148">
+        <v>-2</v>
+      </c>
+      <c r="D148">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A149">
+        <v>1</v>
+      </c>
+      <c r="B149">
+        <v>60</v>
+      </c>
+      <c r="C149">
+        <v>-2</v>
+      </c>
+      <c r="D149">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A150">
+        <v>1</v>
+      </c>
+      <c r="B150">
+        <v>60</v>
+      </c>
+      <c r="C150">
+        <v>-1.6</v>
+      </c>
+      <c r="D150">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A151">
+        <v>1</v>
+      </c>
+      <c r="B151">
+        <v>60</v>
+      </c>
+      <c r="C151">
+        <v>-1.6</v>
+      </c>
+      <c r="D151">
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A152">
+        <v>1</v>
+      </c>
+      <c r="B152">
+        <v>60</v>
+      </c>
+      <c r="C152">
+        <v>-1.6</v>
+      </c>
+      <c r="D152">
+        <v>-1.2</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A153">
+        <v>1</v>
+      </c>
+      <c r="B153">
+        <v>60</v>
+      </c>
+      <c r="C153">
+        <v>-1.6</v>
+      </c>
+      <c r="D153">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A154">
+        <v>1</v>
+      </c>
+      <c r="B154">
+        <v>60</v>
+      </c>
+      <c r="C154">
+        <v>-1.6</v>
+      </c>
+      <c r="D154">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A155">
+        <v>1</v>
+      </c>
+      <c r="B155">
+        <v>60</v>
+      </c>
+      <c r="C155">
+        <v>-1.2</v>
+      </c>
+      <c r="D155">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A156">
+        <v>1</v>
+      </c>
+      <c r="B156">
+        <v>60</v>
+      </c>
+      <c r="C156">
+        <v>-1.2</v>
+      </c>
+      <c r="D156">
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A157">
+        <v>1</v>
+      </c>
+      <c r="B157">
+        <v>60</v>
+      </c>
+      <c r="C157">
+        <v>-1.2</v>
+      </c>
+      <c r="D157">
+        <v>-1.2</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A158">
+        <v>1</v>
+      </c>
+      <c r="B158">
+        <v>60</v>
+      </c>
+      <c r="C158">
+        <v>-1.2</v>
+      </c>
+      <c r="D158">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A159">
+        <v>1</v>
+      </c>
+      <c r="B159">
+        <v>60</v>
+      </c>
+      <c r="C159">
+        <v>-1.2</v>
+      </c>
+      <c r="D159">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A160">
+        <v>1</v>
+      </c>
+      <c r="B160">
+        <v>60</v>
+      </c>
+      <c r="C160">
+        <v>-0.8</v>
+      </c>
+      <c r="D160">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A161">
+        <v>1</v>
+      </c>
+      <c r="B161">
+        <v>60</v>
+      </c>
+      <c r="C161">
+        <v>-0.8</v>
+      </c>
+      <c r="D161">
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A162">
+        <v>1</v>
+      </c>
+      <c r="B162">
+        <v>60</v>
+      </c>
+      <c r="C162">
+        <v>-0.8</v>
+      </c>
+      <c r="D162">
+        <v>-1.2</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A163">
+        <v>1</v>
+      </c>
+      <c r="B163">
+        <v>60</v>
+      </c>
+      <c r="C163">
+        <v>-0.8</v>
+      </c>
+      <c r="D163">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A164">
+        <v>1</v>
+      </c>
+      <c r="B164">
+        <v>60</v>
+      </c>
+      <c r="C164">
+        <v>-0.8</v>
+      </c>
+      <c r="D164">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A165">
+        <v>1</v>
+      </c>
+      <c r="B165">
+        <v>60</v>
+      </c>
+      <c r="C165">
+        <v>-0.4</v>
+      </c>
+      <c r="D165">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A166">
+        <v>1</v>
+      </c>
+      <c r="B166">
+        <v>60</v>
+      </c>
+      <c r="C166">
+        <v>-0.4</v>
+      </c>
+      <c r="D166">
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A167">
+        <v>1</v>
+      </c>
+      <c r="B167">
+        <v>60</v>
+      </c>
+      <c r="C167">
+        <v>-0.4</v>
+      </c>
+      <c r="D167">
+        <v>-1.2</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A168">
+        <v>1</v>
+      </c>
+      <c r="B168">
+        <v>60</v>
+      </c>
+      <c r="C168">
+        <v>-0.4</v>
+      </c>
+      <c r="D168">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A169">
+        <v>1</v>
+      </c>
+      <c r="B169">
+        <v>60</v>
+      </c>
+      <c r="C169">
+        <v>-0.4</v>
+      </c>
+      <c r="D169">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A170">
+        <v>1</v>
+      </c>
+      <c r="B170">
+        <v>120</v>
+      </c>
+      <c r="C170">
+        <v>-2</v>
+      </c>
+      <c r="D170">
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A171">
+        <v>1</v>
+      </c>
+      <c r="B171">
+        <v>120</v>
+      </c>
+      <c r="C171">
+        <v>-2</v>
+      </c>
+      <c r="D171">
+        <v>-1.2</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A172">
+        <v>1</v>
+      </c>
+      <c r="B172">
+        <v>120</v>
+      </c>
+      <c r="C172">
+        <v>-2</v>
+      </c>
+      <c r="D172">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A173">
+        <v>1</v>
+      </c>
+      <c r="B173">
+        <v>120</v>
+      </c>
+      <c r="C173">
+        <v>-2</v>
+      </c>
+      <c r="D173">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A174">
+        <v>1</v>
+      </c>
+      <c r="B174">
+        <v>120</v>
+      </c>
+      <c r="C174">
+        <v>-1.6</v>
+      </c>
+      <c r="D174">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A175">
+        <v>1</v>
+      </c>
+      <c r="B175">
+        <v>120</v>
+      </c>
+      <c r="C175">
+        <v>-1.6</v>
+      </c>
+      <c r="D175">
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A176">
+        <v>1</v>
+      </c>
+      <c r="B176">
+        <v>120</v>
+      </c>
+      <c r="C176">
+        <v>-1.6</v>
+      </c>
+      <c r="D176">
+        <v>-1.2</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A177">
+        <v>1</v>
+      </c>
+      <c r="B177">
+        <v>120</v>
+      </c>
+      <c r="C177">
+        <v>-1.6</v>
+      </c>
+      <c r="D177">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A178">
+        <v>1</v>
+      </c>
+      <c r="B178">
+        <v>120</v>
+      </c>
+      <c r="C178">
+        <v>-1.6</v>
+      </c>
+      <c r="D178">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A179">
+        <v>1</v>
+      </c>
+      <c r="B179">
+        <v>120</v>
+      </c>
+      <c r="C179">
+        <v>-1.2</v>
+      </c>
+      <c r="D179">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A180">
+        <v>1</v>
+      </c>
+      <c r="B180">
+        <v>120</v>
+      </c>
+      <c r="C180">
+        <v>-1.2</v>
+      </c>
+      <c r="D180">
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A181">
+        <v>1</v>
+      </c>
+      <c r="B181">
+        <v>120</v>
+      </c>
+      <c r="C181">
+        <v>-1.2</v>
+      </c>
+      <c r="D181">
+        <v>-1.2</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A182">
+        <v>1</v>
+      </c>
+      <c r="B182">
+        <v>120</v>
+      </c>
+      <c r="C182">
+        <v>-1.2</v>
+      </c>
+      <c r="D182">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A183">
+        <v>1</v>
+      </c>
+      <c r="B183">
+        <v>120</v>
+      </c>
+      <c r="C183">
+        <v>-1.2</v>
+      </c>
+      <c r="D183">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A184">
+        <v>1</v>
+      </c>
+      <c r="B184">
+        <v>120</v>
+      </c>
+      <c r="C184">
+        <v>-0.8</v>
+      </c>
+      <c r="D184">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A185">
+        <v>1</v>
+      </c>
+      <c r="B185">
+        <v>120</v>
+      </c>
+      <c r="C185">
+        <v>-0.8</v>
+      </c>
+      <c r="D185">
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A186">
+        <v>1</v>
+      </c>
+      <c r="B186">
+        <v>120</v>
+      </c>
+      <c r="C186">
+        <v>-0.8</v>
+      </c>
+      <c r="D186">
+        <v>-1.2</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A187">
+        <v>1</v>
+      </c>
+      <c r="B187">
+        <v>120</v>
+      </c>
+      <c r="C187">
+        <v>-0.8</v>
+      </c>
+      <c r="D187">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A188">
+        <v>1</v>
+      </c>
+      <c r="B188">
+        <v>120</v>
+      </c>
+      <c r="C188">
+        <v>-0.8</v>
+      </c>
+      <c r="D188">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A189">
+        <v>1</v>
+      </c>
+      <c r="B189">
+        <v>120</v>
+      </c>
+      <c r="C189">
+        <v>-0.4</v>
+      </c>
+      <c r="D189">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A190">
+        <v>1</v>
+      </c>
+      <c r="B190">
+        <v>120</v>
+      </c>
+      <c r="C190">
+        <v>-0.4</v>
+      </c>
+      <c r="D190">
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A191">
+        <v>1</v>
+      </c>
+      <c r="B191">
+        <v>120</v>
+      </c>
+      <c r="C191">
+        <v>-0.4</v>
+      </c>
+      <c r="D191">
+        <v>-1.2</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A192">
+        <v>1</v>
+      </c>
+      <c r="B192">
+        <v>120</v>
+      </c>
+      <c r="C192">
+        <v>-0.4</v>
+      </c>
+      <c r="D192">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A193">
+        <v>1</v>
+      </c>
+      <c r="B193">
+        <v>120</v>
+      </c>
+      <c r="C193">
+        <v>-0.4</v>
+      </c>
+      <c r="D193">
+        <v>-0.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Converted timing to frames and set up the rest of the trial variables. Configured the stimuli.
</commit_message>
<xml_diff>
--- a/cond-files/cond_pm1.xlsx
+++ b/cond-files/cond_pm1.xlsx
@@ -1,21 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egora\Dropbox\Projects\pm\pm\cond-files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Egor\Dropbox\Projects\pm\pm\cond-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C061406-3572-4263-8D26-E21B7EB03DAA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1234B9EF-7AB5-46CD-8AEC-F3ADEDB9AF7D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="92" yWindow="144" windowWidth="16259" windowHeight="5590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cond_pm1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -900,17 +908,17 @@
   <dimension ref="A1:D193"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A98" sqref="A98:A193"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -1257,10 +1265,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B26">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C26">
         <v>-2</v>
@@ -1271,10 +1279,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B27">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C27">
         <v>-2</v>
@@ -1285,10 +1293,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B28">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C28">
         <v>-2</v>
@@ -1299,10 +1307,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B29">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C29">
         <v>-2</v>
@@ -1313,10 +1321,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B30">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C30">
         <v>-1.6</v>
@@ -1327,10 +1335,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B31">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C31">
         <v>-1.6</v>
@@ -1341,10 +1349,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B32">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C32">
         <v>-1.6</v>
@@ -1355,10 +1363,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B33">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C33">
         <v>-1.6</v>
@@ -1369,10 +1377,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B34">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C34">
         <v>-1.6</v>
@@ -1383,10 +1391,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B35">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C35">
         <v>-1.2</v>
@@ -1397,10 +1405,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B36">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C36">
         <v>-1.2</v>
@@ -1411,10 +1419,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B37">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C37">
         <v>-1.2</v>
@@ -1425,10 +1433,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B38">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C38">
         <v>-1.2</v>
@@ -1439,10 +1447,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B39">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C39">
         <v>-1.2</v>
@@ -1453,10 +1461,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B40">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C40">
         <v>-0.8</v>
@@ -1467,10 +1475,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B41">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C41">
         <v>-0.8</v>
@@ -1481,10 +1489,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B42">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C42">
         <v>-0.8</v>
@@ -1495,10 +1503,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B43">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C43">
         <v>-0.8</v>
@@ -1509,10 +1517,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B44">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C44">
         <v>-0.8</v>
@@ -1523,10 +1531,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B45">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C45">
         <v>-0.4</v>
@@ -1537,10 +1545,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B46">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C46">
         <v>-0.4</v>
@@ -1551,10 +1559,10 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B47">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C47">
         <v>-0.4</v>
@@ -1565,10 +1573,10 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B48">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C48">
         <v>-0.4</v>
@@ -1579,10 +1587,10 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B49">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C49">
         <v>-0.4</v>
@@ -1593,10 +1601,10 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B50">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="C50">
         <v>-2</v>
@@ -1607,10 +1615,10 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B51">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="C51">
         <v>-2</v>
@@ -1621,10 +1629,10 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B52">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="C52">
         <v>-2</v>
@@ -1635,10 +1643,10 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B53">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="C53">
         <v>-2</v>
@@ -1649,10 +1657,10 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B54">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="C54">
         <v>-1.6</v>
@@ -1663,10 +1671,10 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B55">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="C55">
         <v>-1.6</v>
@@ -1677,10 +1685,10 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B56">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="C56">
         <v>-1.6</v>
@@ -1691,10 +1699,10 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B57">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="C57">
         <v>-1.6</v>
@@ -1705,10 +1713,10 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B58">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="C58">
         <v>-1.6</v>
@@ -1719,10 +1727,10 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B59">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="C59">
         <v>-1.2</v>
@@ -1733,10 +1741,10 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B60">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="C60">
         <v>-1.2</v>
@@ -1747,10 +1755,10 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B61">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="C61">
         <v>-1.2</v>
@@ -1761,10 +1769,10 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B62">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="C62">
         <v>-1.2</v>
@@ -1775,10 +1783,10 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B63">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="C63">
         <v>-1.2</v>
@@ -1789,10 +1797,10 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B64">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="C64">
         <v>-0.8</v>
@@ -1803,10 +1811,10 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B65">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="C65">
         <v>-0.8</v>
@@ -1817,10 +1825,10 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B66">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="C66">
         <v>-0.8</v>
@@ -1831,10 +1839,10 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B67">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="C67">
         <v>-0.8</v>
@@ -1845,10 +1853,10 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B68">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="C68">
         <v>-0.8</v>
@@ -1859,10 +1867,10 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B69">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="C69">
         <v>-0.4</v>
@@ -1873,10 +1881,10 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B70">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="C70">
         <v>-0.4</v>
@@ -1887,10 +1895,10 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B71">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="C71">
         <v>-0.4</v>
@@ -1901,10 +1909,10 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B72">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="C72">
         <v>-0.4</v>
@@ -1915,10 +1923,10 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B73">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="C73">
         <v>-0.4</v>
@@ -1929,10 +1937,10 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B74">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="C74">
         <v>-2</v>
@@ -1943,10 +1951,10 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B75">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="C75">
         <v>-2</v>
@@ -1957,10 +1965,10 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B76">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="C76">
         <v>-2</v>
@@ -1971,10 +1979,10 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B77">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="C77">
         <v>-2</v>
@@ -1985,10 +1993,10 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B78">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="C78">
         <v>-1.6</v>
@@ -1999,10 +2007,10 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B79">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="C79">
         <v>-1.6</v>
@@ -2013,10 +2021,10 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B80">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="C80">
         <v>-1.6</v>
@@ -2027,10 +2035,10 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B81">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="C81">
         <v>-1.6</v>
@@ -2041,10 +2049,10 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B82">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="C82">
         <v>-1.6</v>
@@ -2055,10 +2063,10 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B83">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="C83">
         <v>-1.2</v>
@@ -2069,10 +2077,10 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B84">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="C84">
         <v>-1.2</v>
@@ -2083,10 +2091,10 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B85">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="C85">
         <v>-1.2</v>
@@ -2097,10 +2105,10 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B86">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="C86">
         <v>-1.2</v>
@@ -2111,10 +2119,10 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B87">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="C87">
         <v>-1.2</v>
@@ -2125,10 +2133,10 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B88">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="C88">
         <v>-0.8</v>
@@ -2139,10 +2147,10 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B89">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="C89">
         <v>-0.8</v>
@@ -2153,10 +2161,10 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B90">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="C90">
         <v>-0.8</v>
@@ -2167,10 +2175,10 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B91">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="C91">
         <v>-0.8</v>
@@ -2181,10 +2189,10 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B92">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="C92">
         <v>-0.8</v>
@@ -2195,10 +2203,10 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B93">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="C93">
         <v>-0.4</v>
@@ -2209,10 +2217,10 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B94">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="C94">
         <v>-0.4</v>
@@ -2223,10 +2231,10 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B95">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="C95">
         <v>-0.4</v>
@@ -2237,10 +2245,10 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B96">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="C96">
         <v>-0.4</v>
@@ -2251,10 +2259,10 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B97">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="C97">
         <v>-0.4</v>
@@ -2265,10 +2273,10 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B98">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C98">
         <v>-2</v>
@@ -2279,10 +2287,10 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B99">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C99">
         <v>-2</v>
@@ -2293,10 +2301,10 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B100">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C100">
         <v>-2</v>
@@ -2307,10 +2315,10 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B101">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C101">
         <v>-2</v>
@@ -2321,10 +2329,10 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B102">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C102">
         <v>-1.6</v>
@@ -2335,10 +2343,10 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B103">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C103">
         <v>-1.6</v>
@@ -2349,10 +2357,10 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B104">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C104">
         <v>-1.6</v>
@@ -2363,10 +2371,10 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B105">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C105">
         <v>-1.6</v>
@@ -2377,10 +2385,10 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B106">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C106">
         <v>-1.6</v>
@@ -2391,10 +2399,10 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B107">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C107">
         <v>-1.2</v>
@@ -2405,10 +2413,10 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B108">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C108">
         <v>-1.2</v>
@@ -2419,10 +2427,10 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B109">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C109">
         <v>-1.2</v>
@@ -2433,10 +2441,10 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B110">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C110">
         <v>-1.2</v>
@@ -2447,10 +2455,10 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B111">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C111">
         <v>-1.2</v>
@@ -2461,10 +2469,10 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B112">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C112">
         <v>-0.8</v>
@@ -2475,10 +2483,10 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B113">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C113">
         <v>-0.8</v>
@@ -2489,10 +2497,10 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B114">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C114">
         <v>-0.8</v>
@@ -2503,10 +2511,10 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B115">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C115">
         <v>-0.8</v>
@@ -2517,10 +2525,10 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B116">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C116">
         <v>-0.8</v>
@@ -2531,10 +2539,10 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B117">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C117">
         <v>-0.4</v>
@@ -2545,10 +2553,10 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B118">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C118">
         <v>-0.4</v>
@@ -2559,10 +2567,10 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B119">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C119">
         <v>-0.4</v>
@@ -2573,10 +2581,10 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B120">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C120">
         <v>-0.4</v>
@@ -2587,10 +2595,10 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B121">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C121">
         <v>-0.4</v>
@@ -2601,10 +2609,10 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B122">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C122">
         <v>-2</v>
@@ -2615,10 +2623,10 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B123">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C123">
         <v>-2</v>
@@ -2629,10 +2637,10 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B124">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C124">
         <v>-2</v>
@@ -2643,10 +2651,10 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B125">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C125">
         <v>-2</v>
@@ -2657,10 +2665,10 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B126">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C126">
         <v>-1.6</v>
@@ -2671,10 +2679,10 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B127">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C127">
         <v>-1.6</v>
@@ -2685,10 +2693,10 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B128">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C128">
         <v>-1.6</v>
@@ -2699,10 +2707,10 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B129">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C129">
         <v>-1.6</v>
@@ -2713,10 +2721,10 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B130">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C130">
         <v>-1.6</v>
@@ -2727,10 +2735,10 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B131">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C131">
         <v>-1.2</v>
@@ -2741,10 +2749,10 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B132">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C132">
         <v>-1.2</v>
@@ -2755,10 +2763,10 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B133">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C133">
         <v>-1.2</v>
@@ -2769,10 +2777,10 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B134">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C134">
         <v>-1.2</v>
@@ -2783,10 +2791,10 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B135">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C135">
         <v>-1.2</v>
@@ -2797,10 +2805,10 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B136">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C136">
         <v>-0.8</v>
@@ -2811,10 +2819,10 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B137">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C137">
         <v>-0.8</v>
@@ -2825,10 +2833,10 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B138">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C138">
         <v>-0.8</v>
@@ -2839,10 +2847,10 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B139">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C139">
         <v>-0.8</v>
@@ -2853,10 +2861,10 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B140">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C140">
         <v>-0.8</v>
@@ -2867,10 +2875,10 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B141">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C141">
         <v>-0.4</v>
@@ -2881,10 +2889,10 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B142">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C142">
         <v>-0.4</v>
@@ -2895,10 +2903,10 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B143">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C143">
         <v>-0.4</v>
@@ -2909,10 +2917,10 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B144">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C144">
         <v>-0.4</v>
@@ -2923,10 +2931,10 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B145">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C145">
         <v>-0.4</v>
@@ -2937,10 +2945,10 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B146">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="C146">
         <v>-2</v>
@@ -2951,10 +2959,10 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B147">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="C147">
         <v>-2</v>
@@ -2965,10 +2973,10 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B148">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="C148">
         <v>-2</v>
@@ -2979,10 +2987,10 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B149">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="C149">
         <v>-2</v>
@@ -2993,10 +3001,10 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B150">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="C150">
         <v>-1.6</v>
@@ -3007,10 +3015,10 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B151">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="C151">
         <v>-1.6</v>
@@ -3021,10 +3029,10 @@
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B152">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="C152">
         <v>-1.6</v>
@@ -3035,10 +3043,10 @@
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B153">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="C153">
         <v>-1.6</v>
@@ -3049,10 +3057,10 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B154">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="C154">
         <v>-1.6</v>
@@ -3063,10 +3071,10 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B155">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="C155">
         <v>-1.2</v>
@@ -3077,10 +3085,10 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B156">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="C156">
         <v>-1.2</v>
@@ -3091,10 +3099,10 @@
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B157">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="C157">
         <v>-1.2</v>
@@ -3105,10 +3113,10 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B158">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="C158">
         <v>-1.2</v>
@@ -3119,10 +3127,10 @@
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B159">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="C159">
         <v>-1.2</v>
@@ -3133,10 +3141,10 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B160">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="C160">
         <v>-0.8</v>
@@ -3147,10 +3155,10 @@
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B161">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="C161">
         <v>-0.8</v>
@@ -3161,10 +3169,10 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B162">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="C162">
         <v>-0.8</v>
@@ -3175,10 +3183,10 @@
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B163">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="C163">
         <v>-0.8</v>
@@ -3189,10 +3197,10 @@
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B164">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="C164">
         <v>-0.8</v>
@@ -3203,10 +3211,10 @@
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B165">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="C165">
         <v>-0.4</v>
@@ -3217,10 +3225,10 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B166">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="C166">
         <v>-0.4</v>
@@ -3231,10 +3239,10 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B167">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="C167">
         <v>-0.4</v>
@@ -3245,10 +3253,10 @@
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B168">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="C168">
         <v>-0.4</v>
@@ -3259,10 +3267,10 @@
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B169">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="C169">
         <v>-0.4</v>
@@ -3273,10 +3281,10 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B170">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="C170">
         <v>-2</v>
@@ -3287,10 +3295,10 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B171">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="C171">
         <v>-2</v>
@@ -3301,10 +3309,10 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B172">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="C172">
         <v>-2</v>
@@ -3315,10 +3323,10 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B173">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="C173">
         <v>-2</v>
@@ -3329,10 +3337,10 @@
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B174">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="C174">
         <v>-1.6</v>
@@ -3343,10 +3351,10 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B175">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="C175">
         <v>-1.6</v>
@@ -3357,10 +3365,10 @@
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B176">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="C176">
         <v>-1.6</v>
@@ -3371,10 +3379,10 @@
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B177">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="C177">
         <v>-1.6</v>
@@ -3385,10 +3393,10 @@
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B178">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="C178">
         <v>-1.6</v>
@@ -3399,10 +3407,10 @@
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B179">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="C179">
         <v>-1.2</v>
@@ -3413,10 +3421,10 @@
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B180">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="C180">
         <v>-1.2</v>
@@ -3427,10 +3435,10 @@
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B181">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="C181">
         <v>-1.2</v>
@@ -3441,10 +3449,10 @@
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B182">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="C182">
         <v>-1.2</v>
@@ -3455,10 +3463,10 @@
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B183">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="C183">
         <v>-1.2</v>
@@ -3469,10 +3477,10 @@
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B184">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="C184">
         <v>-0.8</v>
@@ -3483,10 +3491,10 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B185">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="C185">
         <v>-0.8</v>
@@ -3497,10 +3505,10 @@
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B186">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="C186">
         <v>-0.8</v>
@@ -3511,10 +3519,10 @@
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B187">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="C187">
         <v>-0.8</v>
@@ -3525,10 +3533,10 @@
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B188">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="C188">
         <v>-0.8</v>
@@ -3539,10 +3547,10 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B189">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="C189">
         <v>-0.4</v>
@@ -3553,10 +3561,10 @@
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B190">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="C190">
         <v>-0.4</v>
@@ -3567,10 +3575,10 @@
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B191">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="C191">
         <v>-0.4</v>
@@ -3581,10 +3589,10 @@
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B192">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="C192">
         <v>-0.4</v>
@@ -3595,10 +3603,10 @@
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B193">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="C193">
         <v>-0.4</v>

</xml_diff>

<commit_message>
Analyses. Planning to switch to location judgment.
</commit_message>
<xml_diff>
--- a/cond-files/cond_pm1.xlsx
+++ b/cond-files/cond_pm1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Egor\Dropbox\Projects\pm\pm\cond-files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egora\Dropbox\Projects\pm\pm\cond-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1234B9EF-7AB5-46CD-8AEC-F3ADEDB9AF7D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5536080-3A78-468F-A09E-4DEDC8435A1C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23263" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cond_pm1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -905,13 +904,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D193"/>
+  <dimension ref="A1:D194"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -938,7 +937,7 @@
         <v>-2</v>
       </c>
       <c r="D2">
-        <v>-1.6</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -952,7 +951,7 @@
         <v>-2</v>
       </c>
       <c r="D3">
-        <v>-1.2</v>
+        <v>-1.6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -966,7 +965,7 @@
         <v>-2</v>
       </c>
       <c r="D4">
-        <v>-0.8</v>
+        <v>-1.2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -980,7 +979,7 @@
         <v>-2</v>
       </c>
       <c r="D5">
-        <v>-0.4</v>
+        <v>-0.8</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -991,10 +990,10 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>-1.6</v>
+        <v>-2</v>
       </c>
       <c r="D6">
-        <v>-2</v>
+        <v>-0.4</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1008,7 +1007,7 @@
         <v>-1.6</v>
       </c>
       <c r="D7">
-        <v>-1.6</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1022,7 +1021,7 @@
         <v>-1.6</v>
       </c>
       <c r="D8">
-        <v>-1.2</v>
+        <v>-1.6</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1036,7 +1035,7 @@
         <v>-1.6</v>
       </c>
       <c r="D9">
-        <v>-0.8</v>
+        <v>-1.2</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -1050,7 +1049,7 @@
         <v>-1.6</v>
       </c>
       <c r="D10">
-        <v>-0.4</v>
+        <v>-0.8</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -1061,10 +1060,10 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <v>-1.2</v>
+        <v>-1.6</v>
       </c>
       <c r="D11">
-        <v>-2</v>
+        <v>-0.4</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -1078,7 +1077,7 @@
         <v>-1.2</v>
       </c>
       <c r="D12">
-        <v>-1.6</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -1092,7 +1091,7 @@
         <v>-1.2</v>
       </c>
       <c r="D13">
-        <v>-1.2</v>
+        <v>-1.6</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -1106,7 +1105,7 @@
         <v>-1.2</v>
       </c>
       <c r="D14">
-        <v>-0.8</v>
+        <v>-1.2</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -1120,7 +1119,7 @@
         <v>-1.2</v>
       </c>
       <c r="D15">
-        <v>-0.4</v>
+        <v>-0.8</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -1131,10 +1130,10 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <v>-0.8</v>
+        <v>-1.2</v>
       </c>
       <c r="D16">
-        <v>-2</v>
+        <v>-0.4</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -1148,7 +1147,7 @@
         <v>-0.8</v>
       </c>
       <c r="D17">
-        <v>-1.6</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -1162,7 +1161,7 @@
         <v>-0.8</v>
       </c>
       <c r="D18">
-        <v>-1.2</v>
+        <v>-1.6</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -1176,7 +1175,7 @@
         <v>-0.8</v>
       </c>
       <c r="D19">
-        <v>-0.8</v>
+        <v>-1.2</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -1190,7 +1189,7 @@
         <v>-0.8</v>
       </c>
       <c r="D20">
-        <v>-0.4</v>
+        <v>-0.8</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -1201,10 +1200,10 @@
         <v>0</v>
       </c>
       <c r="C21">
-        <v>-0.4</v>
+        <v>-0.8</v>
       </c>
       <c r="D21">
-        <v>-2</v>
+        <v>-0.4</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -1218,7 +1217,7 @@
         <v>-0.4</v>
       </c>
       <c r="D22">
-        <v>-1.6</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -1232,7 +1231,7 @@
         <v>-0.4</v>
       </c>
       <c r="D23">
-        <v>-1.2</v>
+        <v>-1.6</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -1246,7 +1245,7 @@
         <v>-0.4</v>
       </c>
       <c r="D24">
-        <v>-0.8</v>
+        <v>-1.2</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -1260,21 +1259,21 @@
         <v>-0.4</v>
       </c>
       <c r="D25">
-        <v>-0.4</v>
+        <v>-0.8</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B26">
         <v>0</v>
       </c>
       <c r="C26">
-        <v>-2</v>
+        <v>-0.4</v>
       </c>
       <c r="D26">
-        <v>-1.6</v>
+        <v>-0.4</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -1288,7 +1287,7 @@
         <v>-2</v>
       </c>
       <c r="D27">
-        <v>-1.2</v>
+        <v>-1.6</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -1302,7 +1301,7 @@
         <v>-2</v>
       </c>
       <c r="D28">
-        <v>-0.8</v>
+        <v>-1.2</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -1316,7 +1315,7 @@
         <v>-2</v>
       </c>
       <c r="D29">
-        <v>-0.4</v>
+        <v>-0.8</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -1327,10 +1326,10 @@
         <v>0</v>
       </c>
       <c r="C30">
-        <v>-1.6</v>
+        <v>-2</v>
       </c>
       <c r="D30">
-        <v>-2</v>
+        <v>-0.4</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -1344,7 +1343,7 @@
         <v>-1.6</v>
       </c>
       <c r="D31">
-        <v>-1.6</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -1358,7 +1357,7 @@
         <v>-1.6</v>
       </c>
       <c r="D32">
-        <v>-1.2</v>
+        <v>-1.6</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -1372,7 +1371,7 @@
         <v>-1.6</v>
       </c>
       <c r="D33">
-        <v>-0.8</v>
+        <v>-1.2</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -1386,7 +1385,7 @@
         <v>-1.6</v>
       </c>
       <c r="D34">
-        <v>-0.4</v>
+        <v>-0.8</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -1397,10 +1396,10 @@
         <v>0</v>
       </c>
       <c r="C35">
-        <v>-1.2</v>
+        <v>-1.6</v>
       </c>
       <c r="D35">
-        <v>-2</v>
+        <v>-0.4</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -1414,7 +1413,7 @@
         <v>-1.2</v>
       </c>
       <c r="D36">
-        <v>-1.6</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -1428,7 +1427,7 @@
         <v>-1.2</v>
       </c>
       <c r="D37">
-        <v>-1.2</v>
+        <v>-1.6</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -1442,7 +1441,7 @@
         <v>-1.2</v>
       </c>
       <c r="D38">
-        <v>-0.8</v>
+        <v>-1.2</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -1456,7 +1455,7 @@
         <v>-1.2</v>
       </c>
       <c r="D39">
-        <v>-0.4</v>
+        <v>-0.8</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -1467,10 +1466,10 @@
         <v>0</v>
       </c>
       <c r="C40">
-        <v>-0.8</v>
+        <v>-1.2</v>
       </c>
       <c r="D40">
-        <v>-2</v>
+        <v>-0.4</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -1484,7 +1483,7 @@
         <v>-0.8</v>
       </c>
       <c r="D41">
-        <v>-1.6</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -1498,7 +1497,7 @@
         <v>-0.8</v>
       </c>
       <c r="D42">
-        <v>-1.2</v>
+        <v>-1.6</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -1512,7 +1511,7 @@
         <v>-0.8</v>
       </c>
       <c r="D43">
-        <v>-0.8</v>
+        <v>-1.2</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -1526,7 +1525,7 @@
         <v>-0.8</v>
       </c>
       <c r="D44">
-        <v>-0.4</v>
+        <v>-0.8</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
@@ -1537,10 +1536,10 @@
         <v>0</v>
       </c>
       <c r="C45">
-        <v>-0.4</v>
+        <v>-0.8</v>
       </c>
       <c r="D45">
-        <v>-2</v>
+        <v>-0.4</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
@@ -1554,7 +1553,7 @@
         <v>-0.4</v>
       </c>
       <c r="D46">
-        <v>-1.6</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
@@ -1568,7 +1567,7 @@
         <v>-0.4</v>
       </c>
       <c r="D47">
-        <v>-1.2</v>
+        <v>-1.6</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
@@ -1582,7 +1581,7 @@
         <v>-0.4</v>
       </c>
       <c r="D48">
-        <v>-0.8</v>
+        <v>-1.2</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -1596,21 +1595,21 @@
         <v>-0.4</v>
       </c>
       <c r="D49">
-        <v>-0.4</v>
+        <v>-0.8</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B50">
         <v>0</v>
       </c>
       <c r="C50">
-        <v>-2</v>
+        <v>-0.4</v>
       </c>
       <c r="D50">
-        <v>-1.6</v>
+        <v>-0.4</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -1624,7 +1623,7 @@
         <v>-2</v>
       </c>
       <c r="D51">
-        <v>-1.2</v>
+        <v>-1.6</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
@@ -1638,7 +1637,7 @@
         <v>-2</v>
       </c>
       <c r="D52">
-        <v>-0.8</v>
+        <v>-1.2</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
@@ -1652,7 +1651,7 @@
         <v>-2</v>
       </c>
       <c r="D53">
-        <v>-0.4</v>
+        <v>-0.8</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
@@ -1663,10 +1662,10 @@
         <v>0</v>
       </c>
       <c r="C54">
-        <v>-1.6</v>
+        <v>-2</v>
       </c>
       <c r="D54">
-        <v>-2</v>
+        <v>-0.4</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -1680,7 +1679,7 @@
         <v>-1.6</v>
       </c>
       <c r="D55">
-        <v>-1.6</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -1694,7 +1693,7 @@
         <v>-1.6</v>
       </c>
       <c r="D56">
-        <v>-1.2</v>
+        <v>-1.6</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
@@ -1708,7 +1707,7 @@
         <v>-1.6</v>
       </c>
       <c r="D57">
-        <v>-0.8</v>
+        <v>-1.2</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
@@ -1722,7 +1721,7 @@
         <v>-1.6</v>
       </c>
       <c r="D58">
-        <v>-0.4</v>
+        <v>-0.8</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
@@ -1733,10 +1732,10 @@
         <v>0</v>
       </c>
       <c r="C59">
-        <v>-1.2</v>
+        <v>-1.6</v>
       </c>
       <c r="D59">
-        <v>-2</v>
+        <v>-0.4</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
@@ -1750,7 +1749,7 @@
         <v>-1.2</v>
       </c>
       <c r="D60">
-        <v>-1.6</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
@@ -1764,7 +1763,7 @@
         <v>-1.2</v>
       </c>
       <c r="D61">
-        <v>-1.2</v>
+        <v>-1.6</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
@@ -1778,7 +1777,7 @@
         <v>-1.2</v>
       </c>
       <c r="D62">
-        <v>-0.8</v>
+        <v>-1.2</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
@@ -1792,7 +1791,7 @@
         <v>-1.2</v>
       </c>
       <c r="D63">
-        <v>-0.4</v>
+        <v>-0.8</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
@@ -1803,10 +1802,10 @@
         <v>0</v>
       </c>
       <c r="C64">
-        <v>-0.8</v>
+        <v>-1.2</v>
       </c>
       <c r="D64">
-        <v>-2</v>
+        <v>-0.4</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
@@ -1820,7 +1819,7 @@
         <v>-0.8</v>
       </c>
       <c r="D65">
-        <v>-1.6</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
@@ -1834,7 +1833,7 @@
         <v>-0.8</v>
       </c>
       <c r="D66">
-        <v>-1.2</v>
+        <v>-1.6</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
@@ -1848,7 +1847,7 @@
         <v>-0.8</v>
       </c>
       <c r="D67">
-        <v>-0.8</v>
+        <v>-1.2</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
@@ -1862,7 +1861,7 @@
         <v>-0.8</v>
       </c>
       <c r="D68">
-        <v>-0.4</v>
+        <v>-0.8</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
@@ -1873,10 +1872,10 @@
         <v>0</v>
       </c>
       <c r="C69">
-        <v>-0.4</v>
+        <v>-0.8</v>
       </c>
       <c r="D69">
-        <v>-2</v>
+        <v>-0.4</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
@@ -1890,7 +1889,7 @@
         <v>-0.4</v>
       </c>
       <c r="D70">
-        <v>-1.6</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
@@ -1904,7 +1903,7 @@
         <v>-0.4</v>
       </c>
       <c r="D71">
-        <v>-1.2</v>
+        <v>-1.6</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
@@ -1918,7 +1917,7 @@
         <v>-0.4</v>
       </c>
       <c r="D72">
-        <v>-0.8</v>
+        <v>-1.2</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
@@ -1932,21 +1931,21 @@
         <v>-0.4</v>
       </c>
       <c r="D73">
-        <v>-0.4</v>
+        <v>-0.8</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B74">
         <v>0</v>
       </c>
       <c r="C74">
-        <v>-2</v>
+        <v>-0.4</v>
       </c>
       <c r="D74">
-        <v>-1.6</v>
+        <v>-0.4</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
@@ -1960,7 +1959,7 @@
         <v>-2</v>
       </c>
       <c r="D75">
-        <v>-1.2</v>
+        <v>-1.6</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
@@ -1974,7 +1973,7 @@
         <v>-2</v>
       </c>
       <c r="D76">
-        <v>-0.8</v>
+        <v>-1.2</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
@@ -1988,7 +1987,7 @@
         <v>-2</v>
       </c>
       <c r="D77">
-        <v>-0.4</v>
+        <v>-0.8</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
@@ -1999,10 +1998,10 @@
         <v>0</v>
       </c>
       <c r="C78">
-        <v>-1.6</v>
+        <v>-2</v>
       </c>
       <c r="D78">
-        <v>-2</v>
+        <v>-0.4</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
@@ -2016,7 +2015,7 @@
         <v>-1.6</v>
       </c>
       <c r="D79">
-        <v>-1.6</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
@@ -2030,7 +2029,7 @@
         <v>-1.6</v>
       </c>
       <c r="D80">
-        <v>-1.2</v>
+        <v>-1.6</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
@@ -2044,7 +2043,7 @@
         <v>-1.6</v>
       </c>
       <c r="D81">
-        <v>-0.8</v>
+        <v>-1.2</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
@@ -2058,7 +2057,7 @@
         <v>-1.6</v>
       </c>
       <c r="D82">
-        <v>-0.4</v>
+        <v>-0.8</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
@@ -2069,10 +2068,10 @@
         <v>0</v>
       </c>
       <c r="C83">
-        <v>-1.2</v>
+        <v>-1.6</v>
       </c>
       <c r="D83">
-        <v>-2</v>
+        <v>-0.4</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
@@ -2086,7 +2085,7 @@
         <v>-1.2</v>
       </c>
       <c r="D84">
-        <v>-1.6</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
@@ -2100,7 +2099,7 @@
         <v>-1.2</v>
       </c>
       <c r="D85">
-        <v>-1.2</v>
+        <v>-1.6</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
@@ -2114,7 +2113,7 @@
         <v>-1.2</v>
       </c>
       <c r="D86">
-        <v>-0.8</v>
+        <v>-1.2</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
@@ -2128,7 +2127,7 @@
         <v>-1.2</v>
       </c>
       <c r="D87">
-        <v>-0.4</v>
+        <v>-0.8</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
@@ -2139,10 +2138,10 @@
         <v>0</v>
       </c>
       <c r="C88">
-        <v>-0.8</v>
+        <v>-1.2</v>
       </c>
       <c r="D88">
-        <v>-2</v>
+        <v>-0.4</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
@@ -2156,7 +2155,7 @@
         <v>-0.8</v>
       </c>
       <c r="D89">
-        <v>-1.6</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
@@ -2170,7 +2169,7 @@
         <v>-0.8</v>
       </c>
       <c r="D90">
-        <v>-1.2</v>
+        <v>-1.6</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
@@ -2184,7 +2183,7 @@
         <v>-0.8</v>
       </c>
       <c r="D91">
-        <v>-0.8</v>
+        <v>-1.2</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
@@ -2198,7 +2197,7 @@
         <v>-0.8</v>
       </c>
       <c r="D92">
-        <v>-0.4</v>
+        <v>-0.8</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
@@ -2209,10 +2208,10 @@
         <v>0</v>
       </c>
       <c r="C93">
-        <v>-0.4</v>
+        <v>-0.8</v>
       </c>
       <c r="D93">
-        <v>-2</v>
+        <v>-0.4</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
@@ -2226,7 +2225,7 @@
         <v>-0.4</v>
       </c>
       <c r="D94">
-        <v>-1.6</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
@@ -2240,7 +2239,7 @@
         <v>-0.4</v>
       </c>
       <c r="D95">
-        <v>-1.2</v>
+        <v>-1.6</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
@@ -2254,7 +2253,7 @@
         <v>-0.4</v>
       </c>
       <c r="D96">
-        <v>-0.8</v>
+        <v>-1.2</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
@@ -2268,21 +2267,21 @@
         <v>-0.4</v>
       </c>
       <c r="D97">
-        <v>-0.4</v>
+        <v>-0.8</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B98">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C98">
-        <v>-2</v>
+        <v>-0.4</v>
       </c>
       <c r="D98">
-        <v>-1.6</v>
+        <v>-0.4</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
@@ -2296,7 +2295,7 @@
         <v>-2</v>
       </c>
       <c r="D99">
-        <v>-1.2</v>
+        <v>-1.6</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
@@ -2310,7 +2309,7 @@
         <v>-2</v>
       </c>
       <c r="D100">
-        <v>-0.8</v>
+        <v>-1.2</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
@@ -2324,7 +2323,7 @@
         <v>-2</v>
       </c>
       <c r="D101">
-        <v>-0.4</v>
+        <v>-0.8</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
@@ -2335,10 +2334,10 @@
         <v>1</v>
       </c>
       <c r="C102">
-        <v>-1.6</v>
+        <v>-2</v>
       </c>
       <c r="D102">
-        <v>-2</v>
+        <v>-0.4</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
@@ -2352,7 +2351,7 @@
         <v>-1.6</v>
       </c>
       <c r="D103">
-        <v>-1.6</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
@@ -2366,7 +2365,7 @@
         <v>-1.6</v>
       </c>
       <c r="D104">
-        <v>-1.2</v>
+        <v>-1.6</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
@@ -2380,7 +2379,7 @@
         <v>-1.6</v>
       </c>
       <c r="D105">
-        <v>-0.8</v>
+        <v>-1.2</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
@@ -2394,7 +2393,7 @@
         <v>-1.6</v>
       </c>
       <c r="D106">
-        <v>-0.4</v>
+        <v>-0.8</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
@@ -2405,10 +2404,10 @@
         <v>1</v>
       </c>
       <c r="C107">
-        <v>-1.2</v>
+        <v>-1.6</v>
       </c>
       <c r="D107">
-        <v>-2</v>
+        <v>-0.4</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
@@ -2422,7 +2421,7 @@
         <v>-1.2</v>
       </c>
       <c r="D108">
-        <v>-1.6</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
@@ -2436,7 +2435,7 @@
         <v>-1.2</v>
       </c>
       <c r="D109">
-        <v>-1.2</v>
+        <v>-1.6</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
@@ -2450,7 +2449,7 @@
         <v>-1.2</v>
       </c>
       <c r="D110">
-        <v>-0.8</v>
+        <v>-1.2</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
@@ -2464,7 +2463,7 @@
         <v>-1.2</v>
       </c>
       <c r="D111">
-        <v>-0.4</v>
+        <v>-0.8</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
@@ -2475,10 +2474,10 @@
         <v>1</v>
       </c>
       <c r="C112">
-        <v>-0.8</v>
+        <v>-1.2</v>
       </c>
       <c r="D112">
-        <v>-2</v>
+        <v>-0.4</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
@@ -2492,7 +2491,7 @@
         <v>-0.8</v>
       </c>
       <c r="D113">
-        <v>-1.6</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
@@ -2506,7 +2505,7 @@
         <v>-0.8</v>
       </c>
       <c r="D114">
-        <v>-1.2</v>
+        <v>-1.6</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
@@ -2520,7 +2519,7 @@
         <v>-0.8</v>
       </c>
       <c r="D115">
-        <v>-0.8</v>
+        <v>-1.2</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
@@ -2534,7 +2533,7 @@
         <v>-0.8</v>
       </c>
       <c r="D116">
-        <v>-0.4</v>
+        <v>-0.8</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
@@ -2545,10 +2544,10 @@
         <v>1</v>
       </c>
       <c r="C117">
-        <v>-0.4</v>
+        <v>-0.8</v>
       </c>
       <c r="D117">
-        <v>-2</v>
+        <v>-0.4</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
@@ -2562,7 +2561,7 @@
         <v>-0.4</v>
       </c>
       <c r="D118">
-        <v>-1.6</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
@@ -2576,7 +2575,7 @@
         <v>-0.4</v>
       </c>
       <c r="D119">
-        <v>-1.2</v>
+        <v>-1.6</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
@@ -2590,7 +2589,7 @@
         <v>-0.4</v>
       </c>
       <c r="D120">
-        <v>-0.8</v>
+        <v>-1.2</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
@@ -2604,21 +2603,21 @@
         <v>-0.4</v>
       </c>
       <c r="D121">
-        <v>-0.4</v>
+        <v>-0.8</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B122">
         <v>1</v>
       </c>
       <c r="C122">
-        <v>-2</v>
+        <v>-0.4</v>
       </c>
       <c r="D122">
-        <v>-1.6</v>
+        <v>-0.4</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
@@ -2632,7 +2631,7 @@
         <v>-2</v>
       </c>
       <c r="D123">
-        <v>-1.2</v>
+        <v>-1.6</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
@@ -2646,7 +2645,7 @@
         <v>-2</v>
       </c>
       <c r="D124">
-        <v>-0.8</v>
+        <v>-1.2</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
@@ -2660,7 +2659,7 @@
         <v>-2</v>
       </c>
       <c r="D125">
-        <v>-0.4</v>
+        <v>-0.8</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
@@ -2671,10 +2670,10 @@
         <v>1</v>
       </c>
       <c r="C126">
-        <v>-1.6</v>
+        <v>-2</v>
       </c>
       <c r="D126">
-        <v>-2</v>
+        <v>-0.4</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
@@ -2688,7 +2687,7 @@
         <v>-1.6</v>
       </c>
       <c r="D127">
-        <v>-1.6</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
@@ -2702,7 +2701,7 @@
         <v>-1.6</v>
       </c>
       <c r="D128">
-        <v>-1.2</v>
+        <v>-1.6</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
@@ -2716,7 +2715,7 @@
         <v>-1.6</v>
       </c>
       <c r="D129">
-        <v>-0.8</v>
+        <v>-1.2</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
@@ -2730,7 +2729,7 @@
         <v>-1.6</v>
       </c>
       <c r="D130">
-        <v>-0.4</v>
+        <v>-0.8</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
@@ -2741,10 +2740,10 @@
         <v>1</v>
       </c>
       <c r="C131">
-        <v>-1.2</v>
+        <v>-1.6</v>
       </c>
       <c r="D131">
-        <v>-2</v>
+        <v>-0.4</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
@@ -2758,7 +2757,7 @@
         <v>-1.2</v>
       </c>
       <c r="D132">
-        <v>-1.6</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
@@ -2772,7 +2771,7 @@
         <v>-1.2</v>
       </c>
       <c r="D133">
-        <v>-1.2</v>
+        <v>-1.6</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
@@ -2786,7 +2785,7 @@
         <v>-1.2</v>
       </c>
       <c r="D134">
-        <v>-0.8</v>
+        <v>-1.2</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
@@ -2800,7 +2799,7 @@
         <v>-1.2</v>
       </c>
       <c r="D135">
-        <v>-0.4</v>
+        <v>-0.8</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
@@ -2811,10 +2810,10 @@
         <v>1</v>
       </c>
       <c r="C136">
-        <v>-0.8</v>
+        <v>-1.2</v>
       </c>
       <c r="D136">
-        <v>-2</v>
+        <v>-0.4</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
@@ -2828,7 +2827,7 @@
         <v>-0.8</v>
       </c>
       <c r="D137">
-        <v>-1.6</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
@@ -2842,7 +2841,7 @@
         <v>-0.8</v>
       </c>
       <c r="D138">
-        <v>-1.2</v>
+        <v>-1.6</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
@@ -2856,7 +2855,7 @@
         <v>-0.8</v>
       </c>
       <c r="D139">
-        <v>-0.8</v>
+        <v>-1.2</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
@@ -2870,7 +2869,7 @@
         <v>-0.8</v>
       </c>
       <c r="D140">
-        <v>-0.4</v>
+        <v>-0.8</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
@@ -2881,10 +2880,10 @@
         <v>1</v>
       </c>
       <c r="C141">
-        <v>-0.4</v>
+        <v>-0.8</v>
       </c>
       <c r="D141">
-        <v>-2</v>
+        <v>-0.4</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
@@ -2898,7 +2897,7 @@
         <v>-0.4</v>
       </c>
       <c r="D142">
-        <v>-1.6</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
@@ -2912,7 +2911,7 @@
         <v>-0.4</v>
       </c>
       <c r="D143">
-        <v>-1.2</v>
+        <v>-1.6</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
@@ -2926,7 +2925,7 @@
         <v>-0.4</v>
       </c>
       <c r="D144">
-        <v>-0.8</v>
+        <v>-1.2</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
@@ -2940,21 +2939,21 @@
         <v>-0.4</v>
       </c>
       <c r="D145">
-        <v>-0.4</v>
+        <v>-0.8</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B146">
         <v>1</v>
       </c>
       <c r="C146">
-        <v>-2</v>
+        <v>-0.4</v>
       </c>
       <c r="D146">
-        <v>-1.6</v>
+        <v>-0.4</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
@@ -2968,7 +2967,7 @@
         <v>-2</v>
       </c>
       <c r="D147">
-        <v>-1.2</v>
+        <v>-1.6</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.3">
@@ -2982,7 +2981,7 @@
         <v>-2</v>
       </c>
       <c r="D148">
-        <v>-0.8</v>
+        <v>-1.2</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.3">
@@ -2996,7 +2995,7 @@
         <v>-2</v>
       </c>
       <c r="D149">
-        <v>-0.4</v>
+        <v>-0.8</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
@@ -3007,10 +3006,10 @@
         <v>1</v>
       </c>
       <c r="C150">
-        <v>-1.6</v>
+        <v>-2</v>
       </c>
       <c r="D150">
-        <v>-2</v>
+        <v>-0.4</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
@@ -3024,7 +3023,7 @@
         <v>-1.6</v>
       </c>
       <c r="D151">
-        <v>-1.6</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
@@ -3038,7 +3037,7 @@
         <v>-1.6</v>
       </c>
       <c r="D152">
-        <v>-1.2</v>
+        <v>-1.6</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
@@ -3052,7 +3051,7 @@
         <v>-1.6</v>
       </c>
       <c r="D153">
-        <v>-0.8</v>
+        <v>-1.2</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
@@ -3066,7 +3065,7 @@
         <v>-1.6</v>
       </c>
       <c r="D154">
-        <v>-0.4</v>
+        <v>-0.8</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
@@ -3077,10 +3076,10 @@
         <v>1</v>
       </c>
       <c r="C155">
-        <v>-1.2</v>
+        <v>-1.6</v>
       </c>
       <c r="D155">
-        <v>-2</v>
+        <v>-0.4</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
@@ -3094,7 +3093,7 @@
         <v>-1.2</v>
       </c>
       <c r="D156">
-        <v>-1.6</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
@@ -3108,7 +3107,7 @@
         <v>-1.2</v>
       </c>
       <c r="D157">
-        <v>-1.2</v>
+        <v>-1.6</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
@@ -3122,7 +3121,7 @@
         <v>-1.2</v>
       </c>
       <c r="D158">
-        <v>-0.8</v>
+        <v>-1.2</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
@@ -3136,7 +3135,7 @@
         <v>-1.2</v>
       </c>
       <c r="D159">
-        <v>-0.4</v>
+        <v>-0.8</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
@@ -3147,10 +3146,10 @@
         <v>1</v>
       </c>
       <c r="C160">
-        <v>-0.8</v>
+        <v>-1.2</v>
       </c>
       <c r="D160">
-        <v>-2</v>
+        <v>-0.4</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.3">
@@ -3164,7 +3163,7 @@
         <v>-0.8</v>
       </c>
       <c r="D161">
-        <v>-1.6</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.3">
@@ -3178,7 +3177,7 @@
         <v>-0.8</v>
       </c>
       <c r="D162">
-        <v>-1.2</v>
+        <v>-1.6</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.3">
@@ -3192,7 +3191,7 @@
         <v>-0.8</v>
       </c>
       <c r="D163">
-        <v>-0.8</v>
+        <v>-1.2</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.3">
@@ -3206,7 +3205,7 @@
         <v>-0.8</v>
       </c>
       <c r="D164">
-        <v>-0.4</v>
+        <v>-0.8</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.3">
@@ -3217,10 +3216,10 @@
         <v>1</v>
       </c>
       <c r="C165">
-        <v>-0.4</v>
+        <v>-0.8</v>
       </c>
       <c r="D165">
-        <v>-2</v>
+        <v>-0.4</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.3">
@@ -3234,7 +3233,7 @@
         <v>-0.4</v>
       </c>
       <c r="D166">
-        <v>-1.6</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.3">
@@ -3248,7 +3247,7 @@
         <v>-0.4</v>
       </c>
       <c r="D167">
-        <v>-1.2</v>
+        <v>-1.6</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.3">
@@ -3262,7 +3261,7 @@
         <v>-0.4</v>
       </c>
       <c r="D168">
-        <v>-0.8</v>
+        <v>-1.2</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.3">
@@ -3276,21 +3275,21 @@
         <v>-0.4</v>
       </c>
       <c r="D169">
-        <v>-0.4</v>
+        <v>-0.8</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B170">
         <v>1</v>
       </c>
       <c r="C170">
-        <v>-2</v>
+        <v>-0.4</v>
       </c>
       <c r="D170">
-        <v>-1.6</v>
+        <v>-0.4</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.3">
@@ -3304,7 +3303,7 @@
         <v>-2</v>
       </c>
       <c r="D171">
-        <v>-1.2</v>
+        <v>-1.6</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.3">
@@ -3318,7 +3317,7 @@
         <v>-2</v>
       </c>
       <c r="D172">
-        <v>-0.8</v>
+        <v>-1.2</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.3">
@@ -3332,7 +3331,7 @@
         <v>-2</v>
       </c>
       <c r="D173">
-        <v>-0.4</v>
+        <v>-0.8</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.3">
@@ -3343,10 +3342,10 @@
         <v>1</v>
       </c>
       <c r="C174">
-        <v>-1.6</v>
+        <v>-2</v>
       </c>
       <c r="D174">
-        <v>-2</v>
+        <v>-0.4</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.3">
@@ -3360,7 +3359,7 @@
         <v>-1.6</v>
       </c>
       <c r="D175">
-        <v>-1.6</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.3">
@@ -3374,7 +3373,7 @@
         <v>-1.6</v>
       </c>
       <c r="D176">
-        <v>-1.2</v>
+        <v>-1.6</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.3">
@@ -3388,7 +3387,7 @@
         <v>-1.6</v>
       </c>
       <c r="D177">
-        <v>-0.8</v>
+        <v>-1.2</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.3">
@@ -3402,7 +3401,7 @@
         <v>-1.6</v>
       </c>
       <c r="D178">
-        <v>-0.4</v>
+        <v>-0.8</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.3">
@@ -3413,10 +3412,10 @@
         <v>1</v>
       </c>
       <c r="C179">
-        <v>-1.2</v>
+        <v>-1.6</v>
       </c>
       <c r="D179">
-        <v>-2</v>
+        <v>-0.4</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.3">
@@ -3430,7 +3429,7 @@
         <v>-1.2</v>
       </c>
       <c r="D180">
-        <v>-1.6</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.3">
@@ -3444,7 +3443,7 @@
         <v>-1.2</v>
       </c>
       <c r="D181">
-        <v>-1.2</v>
+        <v>-1.6</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.3">
@@ -3458,7 +3457,7 @@
         <v>-1.2</v>
       </c>
       <c r="D182">
-        <v>-0.8</v>
+        <v>-1.2</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.3">
@@ -3472,7 +3471,7 @@
         <v>-1.2</v>
       </c>
       <c r="D183">
-        <v>-0.4</v>
+        <v>-0.8</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.3">
@@ -3483,10 +3482,10 @@
         <v>1</v>
       </c>
       <c r="C184">
-        <v>-0.8</v>
+        <v>-1.2</v>
       </c>
       <c r="D184">
-        <v>-2</v>
+        <v>-0.4</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.3">
@@ -3500,7 +3499,7 @@
         <v>-0.8</v>
       </c>
       <c r="D185">
-        <v>-1.6</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.3">
@@ -3514,7 +3513,7 @@
         <v>-0.8</v>
       </c>
       <c r="D186">
-        <v>-1.2</v>
+        <v>-1.6</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.3">
@@ -3528,7 +3527,7 @@
         <v>-0.8</v>
       </c>
       <c r="D187">
-        <v>-0.8</v>
+        <v>-1.2</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.3">
@@ -3542,7 +3541,7 @@
         <v>-0.8</v>
       </c>
       <c r="D188">
-        <v>-0.4</v>
+        <v>-0.8</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.3">
@@ -3553,10 +3552,10 @@
         <v>1</v>
       </c>
       <c r="C189">
-        <v>-0.4</v>
+        <v>-0.8</v>
       </c>
       <c r="D189">
-        <v>-2</v>
+        <v>-0.4</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.3">
@@ -3570,7 +3569,7 @@
         <v>-0.4</v>
       </c>
       <c r="D190">
-        <v>-1.6</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.3">
@@ -3584,7 +3583,7 @@
         <v>-0.4</v>
       </c>
       <c r="D191">
-        <v>-1.2</v>
+        <v>-1.6</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.3">
@@ -3598,7 +3597,7 @@
         <v>-0.4</v>
       </c>
       <c r="D192">
-        <v>-0.8</v>
+        <v>-1.2</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.3">
@@ -3612,6 +3611,20 @@
         <v>-0.4</v>
       </c>
       <c r="D193">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A194">
+        <v>12</v>
+      </c>
+      <c r="B194">
+        <v>1</v>
+      </c>
+      <c r="C194">
+        <v>-0.4</v>
+      </c>
+      <c r="D194">
         <v>-0.4</v>
       </c>
     </row>

</xml_diff>